<commit_message>
Matriz arreglada respecto a arduino, y codigo de prueba de arduino
</commit_message>
<xml_diff>
--- a/ArduinoPromocion/nombres.xlsx
+++ b/ArduinoPromocion/nombres.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
   <si>
     <t xml:space="preserve">Aldo</t>
   </si>
@@ -30,114 +30,117 @@
     <t xml:space="preserve">Ender</t>
   </si>
   <si>
+    <t xml:space="preserve">Gerson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Starky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yeimar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jesus R.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Euro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esteban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antonio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Douglas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nelson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ernesto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Celene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yeinny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Javier C.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Javier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jesus C.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Henry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enmanuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juan F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reyna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maria M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genesis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angelica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrea R.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roxana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freddy</t>
+  </si>
+  <si>
     <t xml:space="preserve">Michael</t>
   </si>
   <si>
-    <t xml:space="preserve">Starky</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yeimar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jesus R.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Euro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esteban</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antonio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Douglas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nelson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ernesto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andrea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Celene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yeinny</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Javier </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Javier C.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Angel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daniel</t>
+    <t xml:space="preserve">Michel</t>
   </si>
   <si>
     <t xml:space="preserve">Jesus</t>
   </si>
   <si>
-    <t xml:space="preserve">Keyla</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Henry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enmanuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juan F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reyna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maria M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erika</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Angelica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genesis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andrea R.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roxana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Freddy</t>
-  </si>
-  <si>
     <t xml:space="preserve">Enmanuel G.</t>
   </si>
   <si>
-    <t xml:space="preserve">Jesus C.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Luis M.</t>
   </si>
   <si>
-    <t xml:space="preserve">Christian</t>
-  </si>
-  <si>
     <t xml:space="preserve">Juan M.</t>
   </si>
   <si>
@@ -180,7 +183,7 @@
     <t xml:space="preserve">Carlos</t>
   </si>
   <si>
-    <t xml:space="preserve">americo</t>
+    <t xml:space="preserve">Americo</t>
   </si>
   <si>
     <t xml:space="preserve">Pietro</t>
@@ -220,8 +223,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -301,7 +305,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -311,6 +315,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -399,118 +407,131 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B64"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B64" activeCellId="0" sqref="B64"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>20</v>
       </c>
@@ -519,236 +540,257 @@
       <c r="A22" s="0" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>36</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>37</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42" s="3"/>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>42</v>
+      </c>
+      <c r="B42" s="4"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>44</v>
+      </c>
+      <c r="B44" s="4"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B48" s="3"/>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>48</v>
+      </c>
+      <c r="B48" s="4"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="B60" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>